<commit_message>
prepping for submission prototype v2
</commit_message>
<xml_diff>
--- a/data/freedom-house/freedom_house_2015.xlsx
+++ b/data/freedom-house/freedom_house_2015.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="12800" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="75">
   <si>
     <t>Status</t>
   </si>
@@ -249,6 +249,9 @@
   </si>
   <si>
     <t>Country</t>
+  </si>
+  <si>
+    <t>Internet_regression</t>
   </si>
 </sst>
 </file>
@@ -563,13 +566,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F66"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="G67" sqref="G67"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>73</v>
       </c>
@@ -588,8 +593,11 @@
       <c r="F1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -608,8 +616,11 @@
       <c r="F2">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2">
+        <v>21.26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -628,8 +639,11 @@
       <c r="F3">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <v>64.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -648,8 +662,11 @@
       <c r="F4">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4">
+        <v>46.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -668,8 +685,11 @@
       <c r="F5">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -688,8 +708,11 @@
       <c r="F6">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -708,8 +731,11 @@
       <c r="F7">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <v>90.998000000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -728,8 +754,11 @@
       <c r="F8">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -748,8 +777,11 @@
       <c r="F9">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9">
+        <v>59.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -768,8 +800,11 @@
       <c r="F10">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10">
+        <v>57.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -788,8 +823,11 @@
       <c r="F11">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -808,8 +846,11 @@
       <c r="F12">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12">
+        <v>87.12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -828,8 +869,11 @@
       <c r="F13">
         <v>40</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13">
+        <v>49.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -848,8 +892,11 @@
       <c r="F14">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14">
+        <v>52.57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -868,8 +915,11 @@
       <c r="F15">
         <v>32</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -888,8 +938,11 @@
       <c r="F16">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -908,8 +961,11 @@
       <c r="F17">
         <v>34</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17">
+        <v>31.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -928,8 +984,11 @@
       <c r="F18">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18">
+        <v>84.24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -948,8 +1007,11 @@
       <c r="F19">
         <v>31</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -968,8 +1030,11 @@
       <c r="F20">
         <v>15</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20">
+        <v>83.75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -988,8 +1053,11 @@
       <c r="F21">
         <v>26</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -1008,8 +1076,11 @@
       <c r="F22">
         <v>11</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G22">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -1028,8 +1099,11 @@
       <c r="F23">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23">
+        <v>86.19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1048,8 +1122,11 @@
       <c r="F24">
         <v>11</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G24">
+        <v>76.13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -1068,8 +1145,11 @@
       <c r="F25">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G25">
+        <v>98.16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -1088,8 +1168,11 @@
       <c r="F26">
         <v>18</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G26">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -1108,8 +1191,11 @@
       <c r="F27">
         <v>19</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G27">
+        <v>17.14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -1128,8 +1214,11 @@
       <c r="F28">
         <v>36</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G28">
+        <v>39.35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -1148,8 +1237,11 @@
       <c r="F29">
         <v>13</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G29">
+        <v>61.96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -1168,8 +1260,11 @@
       <c r="F30">
         <v>11</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30">
+        <v>90.58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -1188,8 +1283,11 @@
       <c r="F31">
         <v>22</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G31">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -1208,8 +1306,11 @@
       <c r="F32">
         <v>24</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G32">
+        <v>54.89</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -1228,8 +1329,11 @@
       <c r="F33">
         <v>13</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G33">
+        <v>43.4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -1248,8 +1352,11 @@
       <c r="F34">
         <v>16</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G34">
+        <v>28.3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -1268,8 +1375,11 @@
       <c r="F35">
         <v>20</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G35">
+        <v>74.7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>38</v>
       </c>
@@ -1288,8 +1398,11 @@
       <c r="F36">
         <v>22</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G36">
+        <v>17.760000000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -1308,8 +1421,11 @@
       <c r="F37">
         <v>13</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G37">
+        <v>5.83</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>40</v>
       </c>
@@ -1328,8 +1444,11 @@
       <c r="F38">
         <v>21</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G38">
+        <v>67.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>41</v>
       </c>
@@ -1348,8 +1467,11 @@
       <c r="F39">
         <v>20</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G39">
+        <v>44.39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -1368,8 +1490,11 @@
       <c r="F40">
         <v>23</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G40">
+        <v>56.8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>43</v>
       </c>
@@ -1388,8 +1513,11 @@
       <c r="F41">
         <v>28</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G41">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>44</v>
       </c>
@@ -1408,8 +1536,11 @@
       <c r="F42">
         <v>15</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G42">
+        <v>42.68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>45</v>
       </c>
@@ -1428,8 +1559,11 @@
       <c r="F43">
         <v>29</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G43">
+        <v>13.8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>46</v>
       </c>
@@ -1448,8 +1582,11 @@
       <c r="F44">
         <v>12</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G44">
+        <v>36.69</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>47</v>
       </c>
@@ -1468,8 +1605,11 @@
       <c r="F45">
         <v>29</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G45">
+        <v>70.52</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>48</v>
       </c>
@@ -1488,8 +1628,11 @@
       <c r="F46">
         <v>19</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G46">
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>49</v>
       </c>
@@ -1508,8 +1651,11 @@
       <c r="F47">
         <v>34</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G47">
+        <v>63.7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>50</v>
       </c>
@@ -1528,8 +1674,11 @@
       <c r="F48">
         <v>21</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G48">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>51</v>
       </c>
@@ -1548,8 +1697,11 @@
       <c r="F49">
         <v>11</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G49">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>52</v>
       </c>
@@ -1568,8 +1720,11 @@
       <c r="F50">
         <v>17</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G50">
+        <v>84.33</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>53</v>
       </c>
@@ -1588,8 +1743,11 @@
       <c r="F51">
         <v>20</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G51">
+        <v>25.8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>54</v>
       </c>
@@ -1608,8 +1766,11 @@
       <c r="F52">
         <v>28</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G52">
+        <v>24.64</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>55</v>
       </c>
@@ -1628,8 +1789,11 @@
       <c r="F53">
         <v>37</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G53">
+        <v>28.09</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>56</v>
       </c>
@@ -1648,8 +1812,11 @@
       <c r="F54">
         <v>32</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G54">
+        <v>34.89</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>57</v>
       </c>
@@ -1668,8 +1835,11 @@
       <c r="F55">
         <v>20</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G55">
+        <v>46.16</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>58</v>
       </c>
@@ -1688,8 +1858,11 @@
       <c r="F56">
         <v>25</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G56">
+        <v>51.04</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>59</v>
       </c>
@@ -1708,8 +1881,11 @@
       <c r="F57">
         <v>18</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G57">
+        <v>17.71</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>60</v>
       </c>
@@ -1728,8 +1904,11 @@
       <c r="F58">
         <v>19</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G58">
+        <v>43.4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>61</v>
       </c>
@@ -1748,8 +1927,11 @@
       <c r="F59">
         <v>32</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G59">
+        <v>90.4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>62</v>
       </c>
@@ -1768,8 +1950,11 @@
       <c r="F60">
         <v>16</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G60">
+        <v>91.61</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>63</v>
       </c>
@@ -1788,8 +1973,11 @@
       <c r="F61">
         <v>14</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G61">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>64</v>
       </c>
@@ -1808,8 +1996,11 @@
       <c r="F62">
         <v>31</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G62">
+        <v>43.55</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>65</v>
       </c>
@@ -1828,8 +2019,11 @@
       <c r="F63">
         <v>22</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G63">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>66</v>
       </c>
@@ -1848,8 +2042,11 @@
       <c r="F64">
         <v>34</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G64">
+        <v>48.31</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>67</v>
       </c>
@@ -1868,8 +2065,11 @@
       <c r="F65">
         <v>17</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G65">
+        <v>17.34</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>68</v>
       </c>
@@ -1887,6 +2087,9 @@
       </c>
       <c r="F66">
         <v>25</v>
+      </c>
+      <c r="G66">
+        <v>19.89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>